<commit_message>
psh to python excel
</commit_message>
<xml_diff>
--- a/testingPs2Py/Services.xlsx
+++ b/testingPs2Py/Services.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,7 +434,24 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Display Name</t>
+          <t>DisplayName</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Running</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>AarSvc_427f0fb</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Agent Activation Runtime_427f0fb</t>
         </is>
       </c>
     </row>
@@ -451,7 +468,41 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Intel® SGX AESM</t>
+          <t>IntelÂ® SGX AESM</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Stopped</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>AJRouter</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>AllJoyn Router Service</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Stopped</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>ALG</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Application Layer Gateway Service</t>
         </is>
       </c>
     </row>

</xml_diff>